<commit_message>
Novos tweets no arquivo principal
</commit_message>
<xml_diff>
--- a/Uber.xlsx
+++ b/Uber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matfs\Desktop\Ciência dos Dados\P2\P1-Classificador-Naive-Bayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A05155F-21DE-408D-907D-E9CD7E30E426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CB6D04-9250-4E6D-800C-7AFC5E13066D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="503">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1066,272 +1066,47 @@
     <t>Teste</t>
   </si>
   <si>
-    <t>rt @grimesimunda: nem td fã do bts é criança! eu, por exemplo, tenho 65 anos, sou mãe de 7 filhos, sou professora, uber, engenheira nuclear…</t>
-  </si>
-  <si>
-    <t>tenho um jobs pra ir aculá mais sem transporte tá difícil, e de uber e nine nine ta dando caríssimo!</t>
-  </si>
-  <si>
-    <t>queria registaram meu ódio pela @uber_brasil de caxias 
-um lixo</t>
-  </si>
-  <si>
-    <t>só hoje eu fiz 5 corridas com a uber, andei mais que notícia ruim</t>
-  </si>
-  <si>
-    <t>as coisas conspiram pra não acreditarem em mim, falei pro bebê que tava na avenida, peguei o uber pra ir pra vila áurea e quem passa de bike? o bebê kkkkkkkkkk</t>
-  </si>
-  <si>
-    <t>tô rindo sozinha lembrando do uber perguntando se docinho era eu kkkkkkk</t>
-  </si>
-  <si>
-    <t>@suzbfr você n mora perto da rafinha? podia fechar um uber vcs, pq ela gosta mas é longe p chegar</t>
-  </si>
-  <si>
-    <t>@cleytxn me diz como minha mãe vai salvar o mundo do coronavirus sendo q ela n sabe nem chamar um uber</t>
-  </si>
-  <si>
-    <t>daí eu teria que pagar um uber pra levar um negócio que nem caixa tem mais e que ta semi montado, gastando mais tempo e mais dinheiro com um erro que não foi meu e sim da loja @leroymerlinbra</t>
-  </si>
-  <si>
-    <t>não culpo o motorista. 
-aqui na minha cidade o taxista consegue levar a cadeira com o porta-malas aberto. 
-se o motorista de app fizer isso, leva multa do guardinha. 
-antigamente eu levava, colocava a cadeira lá atrás, mas agora com gnv não dá mais.
-https://t.co/mqm2ffdjh7</t>
-  </si>
-  <si>
-    <t>@tiagomelo89 @katia58239935 me lembrei do passageiro do uber que sumiu no carro do motorista namorado da maria eduarda... hahahahahaha!</t>
-  </si>
-  <si>
-    <t>@gio_andreotti ah esse uber hj, foi um sinal né</t>
-  </si>
-  <si>
-    <t>como que minha nota no uber ainda ta 5</t>
-  </si>
-  <si>
-    <t>fui entrar no uber e minha mãe veio junto na porta do carro e me pediu tantas vezes pra compartilhar a viagem e avisar quando chegar que o cara fala o tempo todo que tá seguindo o gps kkkkk tadinho</t>
-  </si>
-  <si>
-    <t>@montoale14 esqueci no uber e não consegui recuperar</t>
-  </si>
-  <si>
-    <t>dois carros na garagem e eu indo de uber é nessas horas que fico mais pistola comigo por não saber dirigir</t>
-  </si>
-  <si>
-    <t>rt @coreiafest: motivo 2 - vamos ter muitas pessoas que vão vim de fora, então colocar a resenha logo perto do início da taquaral foi uma e…</t>
-  </si>
-  <si>
-    <t>rt @chicobarney: motorista do uber infelizmente puxando todos os assuntos que tento evitar nos últimos 3 meses (declínio da economia global…</t>
-  </si>
-  <si>
-    <t>é incrível como a #99pop é o dobro da corrida, peço no @uber_brasil e a corrida fica a metade do valor. incrível isso, queria entender a diferença, se a rota é a mesma.</t>
-  </si>
-  <si>
-    <t>@putzz_aninhaa eu falei pra ela qual era o ônibus e o horário mas ela escutou uma menina nova que disse que tinha que pegar outro ônibus 🤦‍♀️ daí viram que tava errado e foram de uber</t>
-  </si>
-  <si>
-    <t>e assim começa a temporada de bizarrice de uber</t>
-  </si>
-  <si>
-    <t>@crladrianin dps o fdp do bruno ficou falando merda dentro do uber kkkkkkkkk</t>
-  </si>
-  <si>
-    <t>@poder360 @jairbolsonaro diz o leitor ou o motorista do uber ?</t>
-  </si>
-  <si>
-    <t>moment white people problrm
-meu uber já errou o caminho 2x 🙄🙄🙄🙄🙄😡😡 eu vou chegar atrasada por causa dessa mula</t>
-  </si>
-  <si>
-    <t>@skycharls ai preciso ir na unimed mas se eu ficar muito tempo no trânsito eu sinto q vou morrer na br dentro do uber hahshahss</t>
-  </si>
-  <si>
-    <t>me amarro em pegar uber black, so carrao</t>
-  </si>
-  <si>
-    <t>pqp n quero pagar isso td de uber</t>
-  </si>
-  <si>
-    <t>tenho q desinstalar uber eats , n ta dando</t>
-  </si>
-  <si>
-    <t>@badbittch_ façamos assim, eu pago o uber e você o resto</t>
-  </si>
-  <si>
-    <t>@serioissoamada eaí @serioissoamada! cupom é sempre bem-vindo na hora da fome né? quer uma dica, fica ligado no nosso app, lá sempre tem um cupom bacana para matar aquela fome. ah! lembrando que você pode compartilhar o seu código com novos amigos para obter desconto.</t>
-  </si>
-  <si>
-    <t>odeio tá no uber atrasa é começar a entrar montão de veículo na frente porra, vontade de falar vai moço bate no carro deles</t>
-  </si>
-  <si>
-    <t>@josielimuniz1 oi, @josielimuniz1! vimos que ainda não segue nossa página. faz o seguinte, segue lá a gente e chama na dm,  assim poderemos te ajudar melhor. https://t.co/sd7yh5jmbj</t>
-  </si>
-  <si>
-    <t>rt @kadu_brandao: passagem de ônibus em salvador r$4,20
-uber para onde quero ir: r$20
-“melhor ir de uber né”</t>
-  </si>
-  <si>
-    <t>rt @o_onivoro: isso acontece quando vc não tem a proteção de leis trabalhistas. provavelmente, era um trabalhador de meio períodos sem dire…</t>
-  </si>
-  <si>
-    <t>o victor hugo só não é mais iludido que eu que pego uma viajem com o uber e to apaixonada</t>
-  </si>
-  <si>
-    <t>rt @_pierresantos: vitor mateus vicente da fonseca, 23 anos, desaparecido em santa catarina aos arredores de são josé/ palhoça, carro encon…</t>
-  </si>
-  <si>
-    <t>e a leticia q pegou um uber em sp com meu cartão e eu aqui desesperado achando q tinha sido clonado...........</t>
-  </si>
-  <si>
-    <t>tive que pedir um uber que ódio caralho que ódio</t>
-  </si>
-  <si>
-    <t>toma lá:
-cupom do ifood (app) =&amp;gt; ee6hz487al
-código rappi =&amp;gt; 82q38640354
-uber -&amp;gt; rjefc5
-r$ 10,00 picpay =&amp;gt; hjsw1z
-99 -&amp;gt; s53bdg5a
-desconto uber eats =&amp;gt; eats-rjefc5
-ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro no perfil! https://t.co/aysqdbarki</t>
-  </si>
-  <si>
-    <t>nos eua, uber lança recurso que envia sms de emergência para a polícia https://t.co/hbq9krzmfr</t>
-  </si>
-  <si>
-    <t>acredito q peguei uber p vir pra aula e n teve chamada</t>
-  </si>
-  <si>
-    <t>baaaaaaah, consegui gastar 500,00 só de uber mês passado, estou de cara 🥵 vlw carnaval</t>
-  </si>
-  <si>
-    <t>rt @irmao_flashofc: duas certezas que carrego comigo:
-1 - jesus vai voltar
-2 - o motorista do uber vai chegar num sandero</t>
-  </si>
-  <si>
-    <t>to num papo cabeça com o uber sobre são caetano.
-no final da corrida acho que eu e ele vamos nos mudar pra lá juntos</t>
-  </si>
-  <si>
-    <t>minha gnt esse uber tem alcool em gel, balinha e lixa de unha to chocada</t>
-  </si>
-  <si>
-    <t>que aplicativo inútil esse @uber_brasil quando se trata de contatar uma central! não tem ninguém pra fazer uma reclamação</t>
-  </si>
-  <si>
-    <t>chegar em casa chamar um uber até a lagoa dos barros sentar na areia ver o por do sol e pensar nos bag</t>
-  </si>
-  <si>
-    <t>pq q o uber tá c 20% de desconto?</t>
-  </si>
-  <si>
-    <t>obrigado uber eats pelo novo mecanismo na hora de confirmar um pedido, o tanto de erro q ja cometi na hora de escolher o método de pagamento não ta escrito 🙏🙏</t>
-  </si>
-  <si>
-    <t>rt @s1ckvitu: partiu usar aquele aplicativo de relacionamento lá, tu marca com a pessoa e depois vai pra um lugar, o tal do uber.</t>
-  </si>
-  <si>
-    <t>@staliniza65 oi, @staliniza65. vamos ajudar vc! antes precisamos que siga a nossa página e depois fale com a gente na dm. te esperamos! https://t.co/sd7yh5jmbj</t>
-  </si>
-  <si>
-    <t>rt @antonybecken: @xetdouber não pode colocar a mão, tem que ser a dobra do braço. esse uber que fuder o país.</t>
-  </si>
-  <si>
-    <t>minha mãe me liga pedindo pra chamar uber pra ela e agora o cel dela descarregou e ela não vai achar o uber, e eu tomo no cu no aplicativo, agora ela tá fudida, nunca mais chamo, tem que aprender a carregar a porra do celular, ou então anda a pé</t>
-  </si>
-  <si>
-    <t>@helo_guedess parcela de um carro já, gastar com uber é mt mina cara</t>
-  </si>
-  <si>
-    <t>só porque eu precisava chegar mais cedo o uber cancela e o outro tá na pqp, 99 n tava funcionando hj</t>
-  </si>
-  <si>
-    <t>@fcksrhai uber tá diferente</t>
-  </si>
-  <si>
-    <t>virei uber de dona fabiana</t>
-  </si>
-  <si>
-    <t>rt @_aurearezende: uber: a
-eu: eh né complicado</t>
-  </si>
-  <si>
-    <t>peguei um uber, o cara super estressado, ele ainda n almoçou, ele esta xingando todo mundo kkkkkkkkkkkkkkkk</t>
-  </si>
-  <si>
-    <t>entrei no uber e tava tocando vitao😍🥰</t>
-  </si>
-  <si>
-    <t>por que leis sobre apps como uber não limitam "precarização" do motorista? https://t.co/gwxeatc9ey via @tilt_uol @uol</t>
-  </si>
-  <si>
-    <t>rt @jennife87309961: eu não sei oq seria de mim se não existisse uber kkk'</t>
-  </si>
-  <si>
-    <t>comprei um negócio p fazer outro negócio e esqueci dentro do uber cara 🤦🏼‍♀️</t>
-  </si>
-  <si>
-    <t>@igortozzi6 @lcnetto @ennzo_mac @vinifernandesdj baforando loló com o uber</t>
-  </si>
-  <si>
-    <t>o cabrini perguntou para cristiana brittes por que ninguém chamou a polícia, ela disse que o celular estava descarregado, então ele fez esta mesma pergunta várias vezes, até que ela diz q o pessoal q estava na casa pediu um uber pra ir embora. 🤦</t>
-  </si>
-  <si>
-    <t>rt @smartinsadv: hoje fiz peguei um @uber_brasil , da pde cacique para centro, 13.34, mot joandre ônix. depois da viagem ele alterou itiner…</t>
-  </si>
-  <si>
-    <t>acabei de pegar um uber que tava com o ar condicionado ligado e com a janela aberta, ai eu peguei e falei que não ia adiantar nada, e ele soltou logo um “vento e ar juntos refrescam mais” kkkkkkkk slk</t>
-  </si>
-  <si>
-    <t>peguei uber mulher e ganhei meu dia 😍</t>
-  </si>
-  <si>
-    <t>algm chama um uber p mim urgente pfvr??</t>
-  </si>
-  <si>
-    <t>olha, tá cada vez mais difícil usar o @uber_brasil quando vc está em um supermercado. motoristas que seguem agindo como se estivessem fazendo um favor ao passageiro, uma falta de simpatia, uma má vontade...</t>
-  </si>
-  <si>
-    <t>rt @jonassritter: @eiviitsii só quem já pediu cigarro no uber eats pra pagar no credito sabe como seria bom</t>
-  </si>
-  <si>
-    <t>o carinha do uber quase bateu o carroo, pqp medo</t>
-  </si>
-  <si>
-    <t>meu deus o uber que eu peguei hoje era filho de italiano 😭😷😷😷</t>
-  </si>
-  <si>
-    <t>@carlazambelli38 uai o bolsonaro não deixou o uber entrar na licitação para atende ele governo em bsb. que ridícula sua posição.</t>
-  </si>
-  <si>
-    <t>@nathan_bezerra1 me transfere 40$
-30$ que o papai te deu
-10$ do uber</t>
-  </si>
-  <si>
-    <t>tenho ranço de uber lesado, vontade de mandar ir p casa do caralho</t>
-  </si>
-  <si>
-    <t>@pepe_takilla falto.... auto propio, taxi o uber. 🤔</t>
-  </si>
-  <si>
-    <t>da minha casa pra de lucas o uber é uns 30/40 reais
-isso quando não era passagem de avião iahsjagah https://t.co/bgg9nzjxho</t>
-  </si>
-  <si>
-    <t>o uber se matando no trap e eu querendo me matar</t>
-  </si>
-  <si>
-    <t>@isabelakarev oi, @isabelakarev! responde a gente na dm, acabamos de falar com você.</t>
-  </si>
-  <si>
-    <t>@therafaamaral não confio em 99 muito menos em uber se não for mulher aí eu vou pq olha tá difícil</t>
-  </si>
-  <si>
-    <t>eu to num uber muito gato mas muito gato muito gato mesmo por favor pare o carro agora e vamos transar</t>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>@mirtuda ri muuito no uber lembrando 😂😂😂
+do nada, e ainda ficaram atolados no chão kkkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>meu deus o uber que meu amigo pegou coitado https://t.co/jm13mai5fj</t>
+  </si>
+  <si>
+    <t>@guga15_ uber mais perfeito não exis....</t>
+  </si>
+  <si>
+    <t>mano kkkkkkkkkk 1x0 pro uber pqp https://t.co/ygbtj7lv8d</t>
+  </si>
+  <si>
+    <t>peguei um uber todo tatuado e escultando um rapzão bem alto, achei q ia ser sequestrada agora</t>
+  </si>
+  <si>
+    <t>expulsas do uber com sucesso kkkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>se agora o sol já está dando moça, imagina na hora que eu for lá pra maiara,  vou chamar um uber isso sim</t>
+  </si>
+  <si>
+    <t>rt @mateus_theus: no final do baile hoje, meu amigo, q por acaso é negro, chamou um uber, e o uber não parou pra ele, daí ele veio todo sem…</t>
+  </si>
+  <si>
+    <t>rt @lugat0: é engraçado que a gente entra na universidade pra supostamente ficar mais inteligente mas cada dia que passa eu só me sinto mai…</t>
+  </si>
+  <si>
+    <t>rt @frente_do_mano3: vem de uber que agnt paga 😈🎈</t>
+  </si>
+  <si>
+    <t>@vikram_giri_28 @shefvaidya ola is uber!</t>
+  </si>
+  <si>
+    <t>com o codigo ubervaledesconto vc ganha muitos creditos na sua conta uber #economize #dinheiro #gratuito #gratis #boaviagem #desconto #crédito #dica #dicadodia #promoção #oferta #viagem #uber #uberx #select #uberselect #black #uberblack #juntos #uberjuntos</t>
+  </si>
+  <si>
+    <t>pegar uber sem me cagar de medo https://t.co/zmvigqpcap</t>
   </si>
   <si>
     <t>cupons de desconto
@@ -1343,22 +1118,755 @@
 p8n9n9smwb - 20 reais no seu primeiro pedido
 99 cupom
 br6e2332 - ganhe 15 reais na sua corrida.
-uber -  vx453h https://t.co/gzirlo0ovp</t>
-  </si>
-  <si>
-    <t>o cara quando vai comprar o carro pra virar uber, o carro já vem com um pendrive lotado de música evangélica pra ficar tocando, é? porra</t>
-  </si>
-  <si>
-    <t>@lpyou_ @therafaamaral mas isso não tem nada com a plataforma... o mesmo motorista da 99, usa uber, tbem. certeza. vai dá índole do motorista.</t>
-  </si>
-  <si>
-    <t>@annupatel77 ola u uber</t>
-  </si>
-  <si>
-    <t>deixei o carro na oficina, e estou indo ao dentista de uber, eu q lute</t>
-  </si>
-  <si>
-    <t>Classe</t>
+uber -  vx453h https://t.co/j3rtkntoyb</t>
+  </si>
+  <si>
+    <t>@suwingando que delícia, da pra ela e deixa eu ser o uber dela</t>
+  </si>
+  <si>
+    <t>tenho vergonha de ir de uber pra essa chácara onde vai ser a calourada pq eh mt ruim de entrar e eu fico kk moço me desculpe eu posso lhe pagar mais se vc quiser kk</t>
+  </si>
+  <si>
+    <t>@rauanyferraz esqueci de te falar que não consegui falar com o uber</t>
+  </si>
+  <si>
+    <t>@apaulazanon @duascoisa @jairbolsonaro @raffaellofazzi é tudo uber #bolsonaroday</t>
+  </si>
+  <si>
+    <t>toda vez que eu vou pra minha tia de uber ele passa por umas ruas tão estranhas que puta que pariu</t>
+  </si>
+  <si>
+    <t>q uber mais sonso
+nossa</t>
+  </si>
+  <si>
+    <t>medo de tossir no uber e ele achar que to com corona</t>
+  </si>
+  <si>
+    <t>rt @marrtinnssss: a bruna pediu um uber pra mim, pq eu tava zero condições, amiga é pra isso kkkkkk</t>
+  </si>
+  <si>
+    <t>@eianjofalacmg manaaaaaa hauahauahaua nera nem pra ter ido, se fosse eu mandava ele meter o uber no cy</t>
+  </si>
+  <si>
+    <t>@brandaodavi_ tbm, passa aqui em casa e a gnt pega um uber</t>
+  </si>
+  <si>
+    <t>mano eu @emillymeneli e @marcosjaquesmj no uber com uns papo de futuro, estudo, trabalho, será-se tamo virando gente? kakaka</t>
+  </si>
+  <si>
+    <t>meu uber tá falando que corona vírus é armação da china pra melhorar a economia dela</t>
+  </si>
+  <si>
+    <t>o auge da minha cachaça: rezar dentro do uber pedindo a deus pra não vomitar dentro do carro. 
+uber: moça mas tá tudo bem? 
+eu: me deixa ta. e ainda se vier noites traiçoeiras se a cruz pesada for</t>
+  </si>
+  <si>
+    <t>@srcartissue oi, @srcartissue. queremos te ajudar a encontrar o item e estamos tentando falar com você na dm, mas ela está bloqueada, pois você não segue nossa página. faz assim, segue nossa página e passa mais detalhes pra gente na dm, assim conseguiremos te ajudar. https://t.co/sd7yh5jmbj</t>
+  </si>
+  <si>
+    <t>queria tossir
+mas tô no uber
+tô c medo do motorista mandar eu descer.kkkkkk</t>
+  </si>
+  <si>
+    <t>ganhei promoção na uber eats e meu hambúrguer veggie vai sair por 7 reais, tô feliz e nao é pouco</t>
+  </si>
+  <si>
+    <t>@milhomem_25 vou te passar o número de um uber amigo pra tu não passar mais por isso gabbie</t>
+  </si>
+  <si>
+    <t>rt @lubrasil: no uber
+-tia o bolsonaro é mau?
+(medo do uber ser minion)
+- barbara , mal não sei, mas ele nao é bom pro nosso país. 
+- tu vo…</t>
+  </si>
+  <si>
+    <t>meu amigo me convencendo da ideia de “uber de sei la oq” que ele não precisa validar e já tem certeza q vai nos deixar ricos // eu https://t.co/jlcqsxwgp5</t>
+  </si>
+  <si>
+    <t>cupom uber março 2020 - ganhe duas corridas na faixa! baixe o aplicativo e use o código: prpon9 https://t.co/g6adtqsw7v</t>
+  </si>
+  <si>
+    <t>olla_0_uber https://t.co/ypncjdtgiw</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/0wvwn7xu4d</t>
+  </si>
+  <si>
+    <t>e o uber que ficava falando que n enxergava direito sem oculos e ficava tirando toda hora p me provar que nao via nada e dirigindo</t>
+  </si>
+  <si>
+    <t>@quirinoalana @ddnr0 kkkkkkk no uber ontem</t>
+  </si>
+  <si>
+    <t>@uber_support obrigadaaaaaaa ♡ mandei tudo por dm!</t>
+  </si>
+  <si>
+    <t>a ari dizendo que pegou um uber e ele bateu o carro kkkkkkk deus eu nunca ri tanto das tragédias desse grupo</t>
+  </si>
+  <si>
+    <t>o dia tá tão lindo vou chamar um uber e ir almoçar na casa de dindinha</t>
+  </si>
+  <si>
+    <t>pessoas em casa não vão usar carros, uber, não vão viajar, consumir, etc. 
+o pior foi ler um relatório de uma casa de research em que eles veem inflação alta como risco no breve horizonte. o cara só pode ser austríaco ou economista da unicamp https://t.co/vpmawxsplm</t>
+  </si>
+  <si>
+    <t>@maluseixass vou pedie uber</t>
+  </si>
+  <si>
+    <t>ta e o uber q deu maconha a nada pra nós ontem, oooo auge nega.</t>
+  </si>
+  <si>
+    <t>se escondendo de epidemia, quase sendo assaltados e o uber não vai pra onde ela mora
+nada é mais são paulo que isso.</t>
+  </si>
+  <si>
+    <t>ontem o uber me chamou delicadamente de pau no cu kkkkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>@marcelo___mello sksksksks gente 
+esquecem andar de uber agora, avaliação 0</t>
+  </si>
+  <si>
+    <t>@aldoreinebr @uber_brasil amrram, agora senta lá amigo</t>
+  </si>
+  <si>
+    <t>lembrei da lavinia e eu cantando thank u next pro cara do uber</t>
+  </si>
+  <si>
+    <t>não vivo sem descontinhos!
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro visite o nosso perfil! https://t.co/uae6qzfga4</t>
+  </si>
+  <si>
+    <t>@ciforosa @herold_dias @karol11_6 @pato_brabo @serieb_br ngm imagina que o filho vai gastar 500$ ou 1000$ em um jogo, a pessoa que usa esses app tipo uber, já deixa o cartão salvo e não espera que o filho vai pedir um carro lá pra outro continente e vc vai ter que pagar milhares de reais por isso kkkkkkk (é só um exemplo)</t>
+  </si>
+  <si>
+    <t>rt @mahlindadetodas: o uber ouvindo esse áudio pela décima vez no dia https://t.co/wlgot0b8fw</t>
+  </si>
+  <si>
+    <t>eu tive que ouvir isso de um uber esses dias e só dei uma risadinha, pois medo de ser morta https://t.co/tm1hjd1px1</t>
+  </si>
+  <si>
+    <t>e vamos de uber eats no próximo mês inteiro...</t>
+  </si>
+  <si>
+    <t>aí eu tava gritando no uber que queria comer, aí implorei pra ele parar pra gente comprar um cachorro quente kkkkkk</t>
+  </si>
+  <si>
+    <t>@xetdouber @_yanfroes @vinicius_cruz7 @_leoarruda0711 @nathanazevd 
+o cara da tucson é uber gente</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/dggypgjasp</t>
+  </si>
+  <si>
+    <t>o cara do uber aí https://t.co/own4v9q7yw</t>
+  </si>
+  <si>
+    <t>obrigado né?
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro no perfil! https://t.co/9jbydz5wzd</t>
+  </si>
+  <si>
+    <t>@guga15_ @upsgabizinha @jessica_syrilo eu se fosse uber</t>
+  </si>
+  <si>
+    <t>do no app, tem o nome do motorista, tem o endereço, cpf, tudo.
+agora se a madame tá lisa e só anda de carro ou você compra o seu, ou você da seu trocado ao motorista de outro app, que provavelmente já foi excluído da uber, só não confunda com o uber</t>
+  </si>
+  <si>
+    <t>@shefvaidya ola oo uber</t>
+  </si>
+  <si>
+    <t>@isabelcrf_ tô no uber wel</t>
+  </si>
+  <si>
+    <t>rt @yves_shiaoi: 1°: entra nas configurações de “sons e tato”
+2°: clica em cima do volume do som que vai aparecer 
+3°: vai tocar o som de l…</t>
+  </si>
+  <si>
+    <t>ontem fui com uma uber pro rolê, conversamos muito sobre ser mulher e o que a gente enfrenta por aí.
+ela me deu o telefone dela e mandou um “menina, não volta muito bebada com homem não tá? se estiver muito bebada pode me ligar, eu te busco onde for, não se coloca em risco” 🥰❤️</t>
+  </si>
+  <si>
+    <t>vindo embora meu primo deu pt no uber affs</t>
+  </si>
+  <si>
+    <t>eu so preciso do video meu e da quel da camila bebadas no uber...</t>
+  </si>
+  <si>
+    <t>eu toda se fosse uber hauahaua @risuenhosz https://t.co/9krguxzgnm</t>
+  </si>
+  <si>
+    <t>@fckjergui gente, o ideal é pedir para uma amiga enviar um áudio se inspirando neste. deixem o áudio favoritado para encontrar com facilidade e usem quando precisar. não acho bom usar esse porque logo ele estará conhecido (até pelos homens uber)</t>
+  </si>
+  <si>
+    <t>única coisa ruim, era o uber, que ficou enchendo saco.</t>
+  </si>
+  <si>
+    <t>uber do boy tá tocando pra caraca, só 5 vezes que tocou foi pra praia ..</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/jmfs4xeeo0</t>
+  </si>
+  <si>
+    <t>entro no uber do nada e fico calculando corrida kkkkkk</t>
+  </si>
+  <si>
+    <t>começar a poupar dessa bateria p uber n é vdd</t>
+  </si>
+  <si>
+    <t>@annaviel_ 15zouu no uber, lindeza</t>
+  </si>
+  <si>
+    <t>rt @wstinglight: alguém sabe se a uber tem uma ouvidoria ou um sac pq eu não encontrei nada no aplicativo</t>
+  </si>
+  <si>
+    <t>pegamos 3 uber ontem, eu fiz amizade com os três 😂😂😂😂 dei meu número e agora me mandaram: bom dia, sou eu o menino do uber 😩 eu nem lembrava disso ☹️</t>
+  </si>
+  <si>
+    <t>a primeira coisa que o uber fala quando eu eu entro é "esqueci que hoje ia ter manifestação pro bolsonaro, se tivesse lembrado eu tinha ido pra lá" e minha única reação foi https://t.co/xibhvkhvrc</t>
+  </si>
+  <si>
+    <t>desgraça uber tá dando 47 conto kkkkkkkkkkkkkkkkkk quero ir mais nn</t>
+  </si>
+  <si>
+    <t>andar com uber que da a seta em cima: 😡😡😡😡😡</t>
+  </si>
+  <si>
+    <t>@jairbolsonaro @edermauropa pelas motos são tudo entregador de ifood é uber tudo pobrezinho kkkkkk https://t.co/omcymgpud9</t>
+  </si>
+  <si>
+    <t>toda vez que ela sai na rua ou entra no uber eu fico preocupado desde da hora em que ela entra até ela sair</t>
+  </si>
+  <si>
+    <t>fiz uma cotação de uber da minha casa até a casa de adriane que é em minas
+deu 1.200
+porraaaa 😂</t>
+  </si>
+  <si>
+    <t>auge do rolê de ontem, @geosccp1910 me leva pra um fim de mundo no meio do nada, dps de sair do caminho de terra um uber passa e da meia volta pra pedi informação. geo:
+- cara, plmds cancela essa corrida e leva a gente pra casa!!</t>
+  </si>
+  <si>
+    <t>peguei um uber ontem na uefs e ele tava usando máscara, tinha um pote enorme de álcool em gel e ele não ligou o ar, vidros abertos. de início minha vontade foi rir por causa da máscara.</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/x50c5wplay</t>
+  </si>
+  <si>
+    <t>o dia de ontem foi tão aleatório eu quase me perdi pq simplesmente quis pegar um uber???</t>
+  </si>
+  <si>
+    <t>rt @atiadeni: ja tomei banho e lavei a mao varias vezes e ainda to vom o cheiro do creme q tava no uber</t>
+  </si>
+  <si>
+    <t>me sentindo culpada por não estar estudando pro enem, mas fui pro banheiro chorar pela nossa situação financeira, juliano n vai poder fazer uber hj pq nem ele nem eu temos dinheiro pra colocar crédito no celular dele, tá faltando coisa em casa, tô mal, chorei e n consigo estudar</t>
+  </si>
+  <si>
+    <t>@0030mary nem me fale amiga kkkkkkkkkkk 30 pau de uber agr pra voltar aí de onde eu saí</t>
+  </si>
+  <si>
+    <t>to indo de uber do multmarket pro prezunic, é muita preguiça mesmo 🤦🏻‍♀️😂</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/0fwvw1czqx</t>
+  </si>
+  <si>
+    <t>@santander_br alô @uber_brasil, agora a bola é com vc. no recibo da viagem (de r$ 13,20) foi descontado os r$ 5,57 de créditos que eu tinha na uber e o resto no meu cartão @santander_br , mas fui ver no meu internet banking que foi descontado os r$ 13,20 (ou seja, o valor integral)</t>
+  </si>
+  <si>
+    <t>uber gostoso do crl meu deus</t>
+  </si>
+  <si>
+    <t>achei que já teriam entendido a dinâmica do negócio depois de tanto tempo usando uber/99.</t>
+  </si>
+  <si>
+    <t>@mcaminhal outras religiões não aceitam jesus nem no@uber</t>
+  </si>
+  <si>
+    <t>amo quando o uber tem bom gosto musical</t>
+  </si>
+  <si>
+    <t>achou! toma aê:
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro visite o nosso perfil! https://t.co/o2jyzafncx</t>
+  </si>
+  <si>
+    <t>eu esqueci por alguns segundos essa parada de corona vírus e dei um puta espirro em cima do uber, sem cobrir nada. coitado, me olhou mt feio</t>
+  </si>
+  <si>
+    <t>@manuuufranco af  e eu q tô em uma resenha n fim do mundo e o ifood n entrega nessa região. tem 3hrs q saíram p buscar pão e nada até agr, daí tô tentando pedir algo pelo uber eats e ifood e nadaaaaaa. foda pq aqui até o isqueiro p acender a churrasqueira esses drogados fdp enfiaram no c*</t>
+  </si>
+  <si>
+    <t>@normose_ olha, eu trabalho como uber e estou super preocupado. minha esposa é transplantada renal e é imunosuprimida. 
+eu preciso trabalhar, mas sei que se apertar demais a doença eu paro mesmo. já reduzi a carga de trabalho, mas saber que tem gente assim me deixa preocupado demais. ai ai</t>
+  </si>
+  <si>
+    <t>rt @jualoeblein: @wjuniormetal fonte: motorista do uber 👍
+#bolsonaroday</t>
+  </si>
+  <si>
+    <t>velho vô escrever uma antologia das experiências vividas no ciará... 
+ontem ao sair à noite bateram no uber q eu tava... 
+o diálogo que se sucedeu foi surreal 😁😜</t>
+  </si>
+  <si>
+    <t>rt @alchemistkkk: utilidade publica 
+use este audio se vc se sentir desconfortavel no uber https://t.co/ym5dotfyhr</t>
+  </si>
+  <si>
+    <t>lembrando aqui que ontem bati a cota de uber, peguei 4 ubers ontem kkkkk</t>
+  </si>
+  <si>
+    <t>merda do corona, eu tinha bue descontos esta semana na uber eats</t>
+  </si>
+  <si>
+    <t>acordei achando que tinha sido um surto mas aí tinha notificação do uber</t>
+  </si>
+  <si>
+    <t>cupom uber março 2020 - ganhe duas corridas na faixa! baixe o aplicativo e use o código: prpon9 https://t.co/tvlnnwxi9d</t>
+  </si>
+  <si>
+    <t>to só as meninas contando que no uber a amara:
+- amiga olha que lindo as luzes da cidade
+e eu respondendo
+- que porra de luz da cidade eu to bebada</t>
+  </si>
+  <si>
+    <t>essas coisas com uber só acontecem comigo mano kkkkkkkkkkkk tnc</t>
+  </si>
+  <si>
+    <t>eu e os guri vamo pegar dois uber pro anima, vou realizar o meu sonho de falar pro uber "siga aquele carro". hoje vai ser afude</t>
+  </si>
+  <si>
+    <t>ontem no uber o motorista falou que o brasil é o lugar mais seguro contra o corona pq tiveram poucos casos confirmados. falei que no estado atual não temos como rastrear o vírus e comentei que uma pessoa que trabalha comigo foi testar pois um amigo da facul deu positivo.</t>
+  </si>
+  <si>
+    <t>@fab1ot chama o uber já !!!!!</t>
+  </si>
+  <si>
+    <t>meu deus eu esqueci meu tênis dentro do uber</t>
+  </si>
+  <si>
+    <t>ontem eu peguei um uber tão legal, a gent foi cantando pagode a viagem inteira</t>
+  </si>
+  <si>
+    <t>de nada pessoal...rs...
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro no nosso perfil https://t.co/nloi2rj7iy</t>
+  </si>
+  <si>
+    <t>@nasudo_157 está fazendo uber po kjjkkkkk</t>
+  </si>
+  <si>
+    <t>kkkkkkkk vítin vomitou o carro do uber todo</t>
+  </si>
+  <si>
+    <t>@arara_ sexta-feira eu estava esperando meu uber na paz de deus pra voltar pra casa e ouvi uma conversa tipo essa e perdi os lados 
+"povo tá chamando o vírus de corona porque só pega coroa, mas o nome científico é covid-19"</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/sj33slzwje</t>
+  </si>
+  <si>
+    <t>eu tava quase conhecendo o outro bairro (as ruas de lá e o caminho da praia pq o resto eu ia de uber rs) dai a gente se mudou pro embare e a unica coisa que agora sei ir é shopping e praia que é perto... e vamos de white people problems avançado</t>
+  </si>
+  <si>
+    <t>tô me sentindo mto mal que ontem dei um calote de 70 centavos no uber. vou ter que dar um calote de 70 reais no zaffari pra me redimir.</t>
+  </si>
+  <si>
+    <t>rt @idareyouagain: chamar uber para foder os cornos a alguém é das coisas mais juliana papada que já vi 
+isto é balongo caralho air force p…</t>
+  </si>
+  <si>
+    <t>uber é uma coisa meio louca né, alguém do nada pensou hummm vou ganhar dinheiro levando a galera para os lugares</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/pvuf92p895</t>
+  </si>
+  <si>
+    <t>e o valor do uber ontem mermão pqp kkkkkkkk, a parada é aqui perto</t>
+  </si>
+  <si>
+    <t>quando é que a glovo ou a uber chega a penafiel ??</t>
+  </si>
+  <si>
+    <t>o uber que eu tô pqp que homem lindooooooo</t>
+  </si>
+  <si>
+    <t>é um tanto egoísta uma pessoa que quase não pega ônibus lotado todos os dias, que não passa por estações de metrô/rodoviárias porque vai pra faculdade de uber, não querer que suspenda as aulas. sem falar que ouvi discursos do tipo: "ah, mas vai atrapalhar minha viagem de julho"</t>
+  </si>
+  <si>
+    <t>@jb_andrade_ @nataamiguel09 que raio de milagre que deu que tu vai? eu vou de uber mas eu moro no tapajós né</t>
+  </si>
+  <si>
+    <t>a raiva q eu tenho de uber q aceita corrida e fica parado</t>
+  </si>
+  <si>
+    <t>rt @tatavoir: armando: 53 anos, tirou essa foto pra colocar de perfil no facebook, compartilha corrente de wpp 
+reginaldo: 50 anos, é moto…</t>
+  </si>
+  <si>
+    <t>@_anahikari @dicas_de_ingles @uber_brasil posts como esse estão ficando bem comum,  poderiam adotar como melhoria no app a opção de cadastro de um número de segurança (opcional). ex. um campo onde eu cadastro o número do meu pai e sempre que inicia uma corrida, automaticamente é enviado as infos importantes.</t>
+  </si>
+  <si>
+    <t>cachaça da perr, fui chamar o uber acabei me cadastrando pra ser motorista kkk</t>
+  </si>
+  <si>
+    <t>to tentando descobrir o nome de um funk que tava tocando no uber ontem quando tava voltando grrrrrrr muito frustrada to ouvindo todas as musicas do top brasil no spotify e nao encontro</t>
+  </si>
+  <si>
+    <t>rt @myxomat00sis: mano e o uber q me disse q o pânico do corona vírus foi criado pela mídia para frustrar as manifestações pró-bolsonaro am…</t>
+  </si>
+  <si>
+    <t>o uber eats me roubando kkkk, baixei o app no cel da minha mãe, usei código de primeira compra, apareceu que foi aplicado e qnd vou comprar aparece o valor normal</t>
+  </si>
+  <si>
+    <t>essa semana eu peguei uber com um italiano:
+eu: o sr tá aqui no brasil há quando tempo?
+ele: cheguei ontem kkkkkk
+eu: ata kk puts
+ele: to zoano boba to aqui há oito anos</t>
+  </si>
+  <si>
+    <t>rt @aafroditeee: meninas cuidado c esse uber! a história é meio longa então quis mostrar tds os detalhes pra q nd fique de fora! 
+(já fiz a…</t>
+  </si>
+  <si>
+    <t>rt @joaobehappy: eu tenho 0 habilidade social para dialogar com uber</t>
+  </si>
+  <si>
+    <t>mano peguei um uber q foi de casa ate o meu trampo fazendo um monteeee de perguntas, basicamente uma consulta, deveria ter cobrado</t>
+  </si>
+  <si>
+    <t>estou lembrando de ontem o uber pedindo o número da minha mãe e ela fingindo que não estava entendendo ,fiquei só olhando pra cara dele 🤦</t>
+  </si>
+  <si>
+    <t>tá tocando thiaguinho no uber, muita felicidade logo cedo</t>
+  </si>
+  <si>
+    <t>@marcelo___mello foda que vc não vai mas poder pedir uber né kkkkk</t>
+  </si>
+  <si>
+    <t>fiz o uber esperar 10mnts só agr ele estar aqui de cr feia kkkkk .. euen</t>
+  </si>
+  <si>
+    <t>e meu uber q ta me levando pra um caminho super diferente vo morre cabo</t>
+  </si>
+  <si>
+    <t>a motorista do uber é uma preta linda que chegou escutando um pagodinho mara.
+meu dia começou do jeito certo</t>
+  </si>
+  <si>
+    <t>pô entrei no uber ontem e virei meu copo nas costa dele cara kkkkkkk mto triste ainda bem q ele é fera</t>
+  </si>
+  <si>
+    <t>o uber passou uma @ maravilhosa pra nois, q rolê viu kkk</t>
+  </si>
+  <si>
+    <t>rt @normose_: acabei de pegar um uber que me assustou. 
+ela disse que 'não vai parar pelo corona precisa trabalhar". segundo ela, um médic…</t>
+  </si>
+  <si>
+    <t>@samyvasconcelos existe amiga, dentro do ifood ou uber eats, só é carro p po**a</t>
+  </si>
+  <si>
+    <t>@_ivojr olá, @_ivojr ! poderia entrar de forma privada e nos informar mais detalhes? https://t.co/sd7yh5jmbj</t>
+  </si>
+  <si>
+    <t>só ontem eu prendi minha mão na porta do uber,quebrei um copo,quebrei uma cadeira, cai no xão 2 vezes</t>
+  </si>
+  <si>
+    <t>alguém sabe se a uber tem uma ouvidoria ou um sac pq eu não encontrei nada no aplicativo</t>
+  </si>
+  <si>
+    <t>uber: que calor eh esse?
+meu pai: pois eh neh 
+*ar co adicionado*: desligado 
+wwwwhaaaaataaaaafuckkkk</t>
+  </si>
+  <si>
+    <t>um uber p barra dando 37 conto fica com deushhhhhhhh</t>
+  </si>
+  <si>
+    <t>imagina só meu pai rodando de uber e passando mal por causa de pressao alta... sem plano de saúde... que maravilha</t>
+  </si>
+  <si>
+    <t>@eduard4pereira_ perdi ontem no uber bb</t>
+  </si>
+  <si>
+    <t>@gabsaraujoo__ vamos?! de uber e baratinho</t>
+  </si>
+  <si>
+    <t>nham nham nham 
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro no perfil! https://t.co/enxjmtsin5</t>
+  </si>
+  <si>
+    <t>isso é tão eu se fosse uber q nem sei https://t.co/am3kvom1tk</t>
+  </si>
+  <si>
+    <t>sair pra rolê e dormir na casa da gabi: não tem problema, já que é 30min da casa dela pra minha, então no uber sai barato.
+sair pra rolê e dormir no apê de gente que conheci faz 1 semana: também não tem problema, mas vou ter que pegar transporte público com essa cara de louca.</t>
+  </si>
+  <si>
+    <t>eu e carla aliviadas de ter pego uber com uma mulher hj cedo dps de assedio de macho escroto a noite toda , foi a gnt q pediu sim</t>
+  </si>
+  <si>
+    <t>ontem a noite minha mãe pediu um uber pra eu ir embora, aí eu fui esperar na rua né pq o uber tava um minuto dali, e o corno por essa enrolação demorou mais de 10 minutos, cmg na rua tendo q ouvir um monte de buzina de macho retardado passando https://t.co/okcznigtpj</t>
+  </si>
+  <si>
+    <t>o uber vc abaixa o preço de viagem, pq a casa da cheirosa e longeee pra carai https://t.co/lejkhpkqs8</t>
+  </si>
+  <si>
+    <t>rt @gcarvalhw: a raiva q eu tenho de uber q aceita corrida e fica parado</t>
+  </si>
+  <si>
+    <t>rt @aline_njpersona: utilidade pública
+áudios e dicas, caso você esteja se sentindo insegura no uber/99 — a thread;
+ https://t.co/i3mvylsv…</t>
+  </si>
+  <si>
+    <t>fui pegar o uber kkkkkk,
+era uma mulher, legal isso</t>
+  </si>
+  <si>
+    <t>estou enviando um desconto de até r$10 em cada uma das suas primeiras 2 viagens com a uber. para aceitar, use o código “sbthaf” ao se cadastrar. aproveite! saiba mais: https://t.co/bqdong18sd</t>
+  </si>
+  <si>
+    <t>@raulveiga esse seu amigo é o cara do uber? 🤔</t>
+  </si>
+  <si>
+    <t>vou tomar um banho me arrumar, e chamar meu uber e foi alvorada</t>
+  </si>
+  <si>
+    <t>@clarobrasil sigo não conseguindo pedir uber, 99 ou entrar no twitter com meu 4g. acabei de verificar minha franquia e só 1 dos 5 gigas de internet foi usado. uso transporte tds dias e ontem me senti super insegura por não conseguir acompanhar a viagem pelo app por conta disso.</t>
+  </si>
+  <si>
+    <t>rt @sosyayayang: vou compartilhar aqui uns videos de tiktokers que fizeram pra vc dar play qnd ta se sentindo desconfortavel no uber/99/etc…</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/yewlugmdx2</t>
+  </si>
+  <si>
+    <t>rt @darkloutommo: meninas olha o que achei no tiktok, é uma nova trend de utilidade pública, caso precisem e estão com medo de pegar uber o…</t>
+  </si>
+  <si>
+    <t>@adrielmarcos9 oi adriel, tudo bem? você já entrou em contato com a uber para verificar se o valor repassado está correto? o cartão é apenas o meio de pagamento.
+peço que verifique com eles e retorne comigo, quero te ajudar.</t>
+  </si>
+  <si>
+    <t>o auge é eu salvando todo e qqr tipo de áudio pra usar no uber pelo simples fato de morrer de medo toda vez q entro em um</t>
+  </si>
+  <si>
+    <t>@arthurmoledoval arthur, para com essa bundamolisse! pqp! 
+pai de família, de verdade . . . precisa pegar ônibus, metrô, precisa se aglomerar nos pontos . . . para trabalhar. você vai fazer o que? criar o bolsa uber?? dizer para os trabalhadores com funções manuais em fábricas fazerem homeoffice?</t>
+  </si>
+  <si>
+    <t>rt @milenesvit: a bárbara espirrando no uber kkkkkkkkkk eu falo logo “moço é corona vírus não viu “</t>
+  </si>
+  <si>
+    <t>acho que se eu fosse uber teria estrela negativa kkkkkk https://t.co/lzftgi56kb</t>
+  </si>
+  <si>
+    <t>[15/3 10:52] fiona👸👭: meu pai vai levar a gente
+[15/3 10:52] fiona👸👭: 🤪.
+[15/3 10:55] amandinha..✨: uffa
+[15/3 10:55] amandinha..✨: amooo
+tenho o melhor tio e o melhor uber 😜</t>
+  </si>
+  <si>
+    <t>eu quero ver como vou falar com meu pai sem a minha madrasta começar com coisa.... sério se ele n puder ele que prepare o bolso pro uber</t>
+  </si>
+  <si>
+    <t>@idalgoo01 desce que o uber tá na porta</t>
+  </si>
+  <si>
+    <t>rt @rommystock: @rucb_chile @florenciare @roquesagrado @ericahenriquezo @cristinauna23 @fridasikahlo @robertofinat @coquiangelica @mahnsa @…</t>
+  </si>
+  <si>
+    <t>@juuhbeeatriiz coronavirus, foi a bala do uber</t>
+  </si>
+  <si>
+    <t>rt @ddemizinho: calor do caralho o corno do motorista do uber com o ar do carro desligado e eu detesto pedir pra ligar</t>
+  </si>
+  <si>
+    <t>rt @t3ddyyyyy: ⚠️ cuidado ⚠️
+muito cuidado ao pegar taxi e uber
+eles estão com carona virus🚗🚕🦠
+😬😬😬😬</t>
+  </si>
+  <si>
+    <t>@santander_br oi @santander_br, então, a foto do recibo (que foi enviado para o meu email após a corrida) que coloquei da minha thread desta conversa, diz que foi cobrado r$ 5,57 dos créditos uber, e o restante do meu cartão, porém, aí ver o meu way, foi descontado o valor integral da viagem</t>
+  </si>
+  <si>
+    <t>tipo meus planos eram apenas fuder gostosinho, fumar um e ir pra casa..........mas acabei indo pro desvio (que tava vazio vai se fuder corona virus), voltei pra casa bebado e batendo altos papos com o uber</t>
+  </si>
+  <si>
+    <t>o uber desabando comigo sobre a ex mulher e a atual kkkkkkkkkkklkk coitado, to nem resolvendo minha vida</t>
+  </si>
+  <si>
+    <t>o quão adolescente padrão você é?
+tem netflix: 👎
+tem spotify: 👍
+tem telecine p: 👎
+tem crush: 👍
+tem mais de 5 amgs:👍
+é popular: 👎
+tem iphone: 👎
+tem android: 👍
+tem mais de 1,50: 👍
+é mimade: 👎👍
+a família é unida:👍👎
+tem um quarto só seu: 👎
+anda de uber: 👎 https://t.co/t90jyzdzpi</t>
+  </si>
+  <si>
+    <t>conheci um guri ontem q era uber e eu jurava q ele ia me sequestrar</t>
+  </si>
+  <si>
+    <t>calor do caralho o corno do motorista do uber com o ar do carro desligado e eu detesto pedir pra ligar</t>
+  </si>
+  <si>
+    <t>neste tempo de crise, não peçam uber eats, glovo ou estafetas desse tipo. se vocês não querem sair de casa, os estafetas não têm outro remédio. e não se esqueçam que eles podem contactar com dezenas de pessoas antes de vos baterem à porta. o vosso menu pode vir com extra corona.</t>
+  </si>
+  <si>
+    <t>@gabiivieirar @uber_brasil eu liguei pra ele, ele desligou na minha cara, ele olhou casa mensagem q eu mandei, só finalizou quando eu liguei mais de 10 vezes pra ele</t>
+  </si>
+  <si>
+    <t>o uber brotando no rolê ontem pra saber se eu tava bem kkkkkkkkk</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/zpgienji5b</t>
+  </si>
+  <si>
+    <t>@superahnega coisa de qm chega de madrugada me olha e não desce do uber</t>
+  </si>
+  <si>
+    <t>@detergenteveja entrei em depreso ontem naquele uber</t>
+  </si>
+  <si>
+    <t>vc quer então toma lá:
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro no nosso perfil https://t.co/gz7g334hol</t>
   </si>
 </sst>
 </file>
@@ -1772,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E304" sqref="E304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1786,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>389</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4198,450 +4706,1624 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A88"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="255.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>388</v>
+        <v>389</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>390</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>391</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>392</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>393</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>394</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>395</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>396</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>397</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>398</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>399</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>400</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>401</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>402</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>403</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>404</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>405</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>406</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>407</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>408</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>409</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>410</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>411</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>412</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>413</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>414</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>415</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>416</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>417</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>418</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>419</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>420</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>421</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>422</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>423</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>424</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>425</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>426</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>427</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>428</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>429</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>430</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>431</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>432</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>433</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>434</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>435</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>436</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>437</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>438</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>439</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>440</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>441</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>442</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>443</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>444</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>445</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>446</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>447</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>448</v>
+      </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>449</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>450</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>451</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>452</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>453</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>454</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>455</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>456</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>457</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>458</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>459</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>460</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>461</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>462</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>463</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>464</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>465</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>466</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>467</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>468</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>469</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>470</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>471</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>472</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>473</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>474</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>475</v>
+      </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>476</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>477</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>478</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>479</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>480</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>481</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>482</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>483</v>
+      </c>
+      <c r="B182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>484</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>485</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>486</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>487</v>
+      </c>
+      <c r="B186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>488</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>489</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>490</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>491</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>492</v>
+      </c>
+      <c r="B191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>493</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>494</v>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>495</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>496</v>
+      </c>
+      <c r="B195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>497</v>
+      </c>
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>498</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>499</v>
+      </c>
+      <c r="B198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>500</v>
+      </c>
+      <c r="B199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>501</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>502</v>
+      </c>
+      <c r="B201">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionei mais tweets à base de treinamento
</commit_message>
<xml_diff>
--- a/Uber.xlsx
+++ b/Uber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matfs\Desktop\Ciência dos Dados\P2\P1-Classificador-Naive-Bayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CB6D04-9250-4E6D-800C-7AFC5E13066D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B634194-A582-498D-BC29-78B5AAC89D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="703">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1867,6 +1867,792 @@
 99 (carona) -&amp;gt; s53bdg5a
  desconto uber eats =&amp;gt; eats-rjefc5
 ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro no nosso perfil https://t.co/gz7g334hol</t>
+  </si>
+  <si>
+    <t>a porra do uber eats chegou na minha cidade mas não entrega no meu bairro https://t.co/fu5oo49phj</t>
+  </si>
+  <si>
+    <t>olha a chuva de descontinhos:
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro visite o nosso perfil! https://t.co/f1ohzbbkit</t>
+  </si>
+  <si>
+    <t>rt @pegoncalves: o uber se protegendo com plastico é maravilhoso demais.
+viva o brasileiro https://t.co/wxp7rhgvwd</t>
+  </si>
+  <si>
+    <t>pagar 30$ de uber 
+pegar 4 ônibus que demora praticamente 3h pra chegar 
+é algum sinal de amor ? aiai</t>
+  </si>
+  <si>
+    <t>qnd minha mãe falar que ta entrando no uber pra vim embora, eu levanto pra arrumar a casa 😂</t>
+  </si>
+  <si>
+    <t>galera vcs q andam de uber, qual o problema pessoal que vocês têm com o tapete do meu carro??????????????????</t>
+  </si>
+  <si>
+    <t>rt @carlosrochape: será que alguém pode me ajudar???
+algum de vcs sabem onde esse cidadão de nome tarciso, motorista de uber reside(mora)?…</t>
+  </si>
+  <si>
+    <t>a gente sabe q o negócio tá um absurdo quando vê mulheres ter que usar áudios falsos pra se sentir seguras dentro de um uber https://t.co/qrpamnw1m9</t>
+  </si>
+  <si>
+    <t>@hajiketobiume ta loco tinha q rushar um mes de uber eats de bike so pra apreciar esses jogos depois kkkkkk</t>
+  </si>
+  <si>
+    <t>eu de uber https://t.co/gdrqtmq83h</t>
+  </si>
+  <si>
+    <t>minha mãe: "ó, vou dar uma saidinha mas se alguma das panela de pressão fizer barulho de explodir, você desliga o fogo, tá?"
+rapaz, se essa panela fizer um barulho a mais eu tô pegando um uber pra cidade vizinha</t>
+  </si>
+  <si>
+    <t>nossa é mt triste ter áudio pra ouvir no uber quando tem medo de ser abusada.... isso é mt triste! https://t.co/fiopzgxinr</t>
+  </si>
+  <si>
+    <t>e o vitinho que resolveu pegar um uber cm os carvão quente dentro do acendedor, q q deu? caiu no banco e quase pegou fogo no carro inteiro kkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>ou que ficasse pensando em como ganharia a vida, porque estava trabalhando por conta há cinco anos, como motorista de uber, devido à um corte de funcionários em sua antiga empresa. como motorista, ele saberia que estaria sozinho nessa.</t>
+  </si>
+  <si>
+    <t>o uber do neo fascismo ! convoca o gado para em plena pandemia se concentrarem em todo país !! esses imbecís merecem o pior !! são além de antidemocratas um grandes imbecis 🦠#bolsonaroday #bolsonarocorno #forabolsonaro https://t.co/d0wfzolguk</t>
+  </si>
+  <si>
+    <t>meu pai q foi pedalando até o poço azul e não consegue mais pedalar kkkkkkkkkkkkkkk coitado 
+to tentando pedir um uber pra ele, mas não tem nenhum disponível</t>
+  </si>
+  <si>
+    <t>rt @kookzvmin: taekook au
+onde jungkook estava atrasado para uma prova importantíssima e acaba por pedir um uber porém enquanto esperava p…</t>
+  </si>
+  <si>
+    <t>uber eats eu te odeio</t>
+  </si>
+  <si>
+    <t>@allantercalivre o carnaval tava suave 🙄
+q gente hipócrita pqp!
+por favor não pegue ônibus.. metrô.. uber viu! 👍🏻</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/yk6bb7m7qp</t>
+  </si>
+  <si>
+    <t>pra começar bem a semana tô achando que deixei meu carregador dentro do carro do uber... e eu ainda coloquei ele no meu colo.</t>
+  </si>
+  <si>
+    <t>rt @galegomatheus1: imagina isso: 
+vc é motorista do uber e sente um movimento estranho no banco de trás 
+daí vc olha pelo retrovisor e dá…</t>
+  </si>
+  <si>
+    <t>cara eu acho tao horrivel que a gnt tem que usar isso pra se sentir segura ou no minimo nao ser sla sequestrada ou estuprada pelo uber tipo?????? e tem gente q fala q feminismo é mimimi tipo quando q algum mlk ficou com medo de pegar uber? nunca. https://t.co/fjanvzhirq</t>
+  </si>
+  <si>
+    <t>chamar uber para foder os cornos a alguém é das coisas mais juliana papada que já vi 
+isto é balongo caralho air force preta gang gang https://t.co/vs3tiuhdbc</t>
+  </si>
+  <si>
+    <t>aquele tipo de uber que quando você pede ele vai lavando sua roupa durante a viagem
+o uber comfort</t>
+  </si>
+  <si>
+    <t>meu pai patrocinou meu uber, óó gloria 🙏🏽🙏🏽</t>
+  </si>
+  <si>
+    <t>rt @dudabias: cara????? e meu namorado???  q decidiu rodar no uber, eis o resultado: https://t.co/4pzjq10b7z</t>
+  </si>
+  <si>
+    <t>rt @studyaugusto: thread com áudios pra você usar quando se sentir desconfortável no uber!
+✨de rt porque você pode impedir que pessoas sof…</t>
+  </si>
+  <si>
+    <t>ooo esse cara do uber véi 🤣🤣🤣🤣</t>
+  </si>
+  <si>
+    <t>o uber falando que mulher q presta eles homens não gostam, aquelas q ficam no pé eles não querem, p tu ver né kkkkkkk</t>
+  </si>
+  <si>
+    <t>rt @omardeideais: o uber agora falando de privatização, eu:
+- claro, tem que privatizar tudo.
+- tudo!
+- até a saúde, que se foda. bom qu…</t>
+  </si>
+  <si>
+    <t>cupom uber março 2020 - ganhe duas corridas na faixa! baixe o aplicativo e use o código: prpon9 https://t.co/npmwqhsufv</t>
+  </si>
+  <si>
+    <t>queria cupom do uber eats</t>
+  </si>
+  <si>
+    <t>rt @hannahadama: cara eu to muito triste com oq acabou de acontecer, simplesmente uma moça aterrorizada chegou na minha amiga pedindo ajuda…</t>
+  </si>
+  <si>
+    <t>esse uber enrola p crl🙄</t>
+  </si>
+  <si>
+    <t>me sentindo abençoada por só estar pegando uber com motorista mulher 🥰🥰🥰 obg deus por me sondar</t>
+  </si>
+  <si>
+    <t>eu se fosse uber 😂😂😂😂 https://t.co/lq1qv5q2cw</t>
+  </si>
+  <si>
+    <t>ontem pedir um uber pra buscar mikaelly, quando ele deixou ela em casa, ele me mandou msg dizendo que ela tá já tava em casa kkk tipo, ele deu pra perceber a preocupação e o amor q tenho por essa garota, por mais q ela me pertuba até me estressar não vivo sem ❤️ @feliciomikaelly</t>
+  </si>
+  <si>
+    <t>complicado 
+falei pra minha mae que sou a uber privada dela https://t.co/goovyaao90</t>
+  </si>
+  <si>
+    <t>@bellasoarez oi, @bellasoarez. vamos ajudar você a descolar esse almoço! segue essa página aqui e chama na dm com mais detalhes sobre a situação que vamos verificar. https://t.co/sd7yh5ax3h</t>
+  </si>
+  <si>
+    <t>acordei no chao do lado da cama usando um moletom como se fosse calça e esqueci meu oculos no uber</t>
+  </si>
+  <si>
+    <t>@thiifate ahhhh quer dizer então que o sr presidente bolsonaro ao lado de um alemão invoca a situação se nazifascista.... hummm, quando vc for pegar um uber e o carro for um volkswagen saia correndo... não entre...</t>
+  </si>
+  <si>
+    <t>voce se sente um lixo, quando vê que as manas tem que usar um vídeo falso pra se sentir menos desconfortável no uber... sério to revoltada https://t.co/wfps5tt1xq</t>
+  </si>
+  <si>
+    <t>rt @gdegustav: @monaurr @lucasleonardoa o uber depois de ouvir vários áudios de passageiras diferentes falando a mesma coisa e falando que…</t>
+  </si>
+  <si>
+    <t>o uber n acreditou q eu tenho 14 anos e perguntou se eu namorava 
+entrei em c h o q u e</t>
+  </si>
+  <si>
+    <t>@iriss_gomes piris paga um uber pra mim</t>
+  </si>
+  <si>
+    <t>não sei como não morri dentro desse uber ainda</t>
+  </si>
+  <si>
+    <t>rt @_caralice: coé galera
+com essa pandemia do coronavírus, meu irmão que é uber tá com uma demanda muito menor de trabalho
+ele é provedor…</t>
+  </si>
+  <si>
+    <t>@surviv0rr senhor, de uber é tão rapidinho :(</t>
+  </si>
+  <si>
+    <t>quem sou eu salvando todos os áudios pra usar quando tiver no uber</t>
+  </si>
+  <si>
+    <t>ontem tive a sensatez de ir embora enquanto o uber tava barato</t>
+  </si>
+  <si>
+    <t>a foto do meu uber é totalmente conceitual</t>
+  </si>
+  <si>
+    <t>kkkkkkkkkkkkkkkk tô rindo de ódio! olha só @uber_brasil como seus clientes são tratados! pf ajudem na transmissão desta mensagem. 
+ #uberoportunista #sovisalucro
+#nosquepaguemosaconta https://t.co/hmu14k5qh0</t>
+  </si>
+  <si>
+    <t>a anna pedindo o uber no meio da madrugada pq não aguentava mais eu, fernanda e murilo tentando aprender a coreografia de desliza e joga https://t.co/csvpzg5ais</t>
+  </si>
+  <si>
+    <t>@fariamoney entrei em contato com o nubank que acho que eles vão resolver mais rápido kkkkkk se não der certo ainda eu falo com a uber</t>
+  </si>
+  <si>
+    <t>meu deus não aguento mais essa musica que a uber tá escutando 🤦🏻‍♀️</t>
+  </si>
+  <si>
+    <t>peguei um uber tão gente boa ontem 
+a conversa fluiu tão bem</t>
+  </si>
+  <si>
+    <t>eu e o uber ouvindo o jogo e falando mal do grêmio. time desgraçado 🤦🏼‍♀️</t>
+  </si>
+  <si>
+    <t>coloquei o fone, mas to com medo dele falar cmg e eu não escutar aaaaaaa uber pq tão fofo</t>
+  </si>
+  <si>
+    <t>@toom_ @funceme minha meta tá dando certo. fazer com que vc se sinta ruim por usar uber! 😴</t>
+  </si>
+  <si>
+    <t>@glaubermacario @reginamorli @barbaragancia aposto que ela é uber e acredita que é "patroa de si mesma", coitada.</t>
+  </si>
+  <si>
+    <t>o uber de 10 reais virou 20 por causa da rua alagada https://t.co/hhpwbune3j</t>
+  </si>
+  <si>
+    <t>me preparando pra ir pra belford roxo kkkkkk vai ser só quase uma hora pra conseguir uber. mas hoje é dia de comemorar com a florzinha ❤️</t>
+  </si>
+  <si>
+    <t>vim tentando falar com o uber mas o cara me ignorou total, só fazia uhum com a cabeça</t>
+  </si>
+  <si>
+    <t>@lorranycarioca reclama na uber, ele não pode me mesmo te cobrar uma corrida pq você esqueceu sua sandália</t>
+  </si>
+  <si>
+    <t>rt @danieloguerra2: ei isso daq foi genial boe.
+usem caso não se sintam confortáveis no uber! nos comentários tem uma versão masculina até…</t>
+  </si>
+  <si>
+    <t>gente, e eu que falei “e vamos de bom dia” pro uber</t>
+  </si>
+  <si>
+    <t>@_nandsdias achei, mas só conseguimos falar com o uber de tarde, foi um rolê kkkkk</t>
+  </si>
+  <si>
+    <t>o hiago falando do carro capotando na lombada da br e depois de 10s quase acontece com a gente dentro do uber kkkkdkdkkk</t>
+  </si>
+  <si>
+    <t>meu uber me tranquilizou total sobre o corona, ele disse que era assim mesmo: de tempos em tempos a população mundial precisa ser quase que completamente dizimada p não inchar.... ...
+ok...</t>
+  </si>
+  <si>
+    <t>rt @gaabipoli: a gente pega cada uber, não da pra acreditar kkkkkkkk</t>
+  </si>
+  <si>
+    <t>cara do uber espirrou e o carro tá fechado por causa do ar meu deus</t>
+  </si>
+  <si>
+    <t>pagando micao c o uber ontem 😚✌🏻✌🏻</t>
+  </si>
+  <si>
+    <t>@kaylanecrf3 e muito confortável pegar uber mulher</t>
+  </si>
+  <si>
+    <t>mano bebi tanto que nem sei como conseguir chegar em casa se não fosse o uber eu nem sei rs,</t>
+  </si>
+  <si>
+    <t>o uber é boiola obrigado old q vou *****</t>
+  </si>
+  <si>
+    <t>@santander_br mas irei ver direitinho sobre isso com a @uber_brasil!</t>
+  </si>
+  <si>
+    <t>motorista do uber cantando pagode na maior alegria 11 da manhã é tudo pra mim 🥺</t>
+  </si>
+  <si>
+    <t>fds vou de uber pra turvo</t>
+  </si>
+  <si>
+    <t>bah, o uber dela tá vindo de ré</t>
+  </si>
+  <si>
+    <t>ola hu uber... 🤣😂 https://t.co/zjwp4cshag</t>
+  </si>
+  <si>
+    <t>@olimpiabarbara @uber_brasil e se fala q vai denunciar, o cara ainda fica puto, não entendo esses uber q não querem trabalhar direito, é só sair do app e deixa quem realmente quer</t>
+  </si>
+  <si>
+    <t>@anabarbara_leal eu tava cvs com o uber ,nem no zap na vdd eu entrei</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/asfq9zw0em</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/auew40a7tx</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/w01fpprrcj</t>
+  </si>
+  <si>
+    <t>seja esperto e coma com o descontinho!
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas amazon, airbnb, recargapay, mercado livre, pagseguro lá no perfil! https://t.co/s9i7dhlplq</t>
+  </si>
+  <si>
+    <t>@geosccp1910  falando cm o uber:
+- moss, o jeito q vc deu meia volta ali, se eu tivesse uma arma c ja tava morto! 
+kkkkkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>minha irma é uber né, daí ela contou a seguinte conversa que teve com um passageiro que pegou em um evento ontem 
+ela: tá muito cheio aí?
+ele: tá lotado 
+ela: mas não tá com medo do corona não?
+ele: morre com álcool né e eu bebo pra caralho 
+manoooo kakaakakakaka</t>
+  </si>
+  <si>
+    <t>ah se todos os uber fossem assim... eu andaria sempre de uber https://t.co/zx37qif7ff</t>
+  </si>
+  <si>
+    <t>quando cancelamos uma corrida somos punidos, pagamos pelo cancelamento, mas qdo os motoristas nos constrangem nos obrigando a dizer pra onde vamos, cancelam a corrida s. nenhum motivo, fato é q nem temos como abrir uma reclamação, né @uber_brasil? há punição pra eles(motorista)?</t>
+  </si>
+  <si>
+    <t>@beca_nobres3 e tu gritando no uber ainda kkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>@acabraquele @delucca e quando é autônomo? uber?</t>
+  </si>
+  <si>
+    <t>@vitornoisvai @uber_brasil eu tive que desinstalar o app, pq quase 22h já e o cara não tinha cancelado, só rodando.
+sorte que eu consegui recorrer dps.</t>
+  </si>
+  <si>
+    <t>@santander_br @uber_brasil eu tô meio perdido para a solução. não sei se a @santander_br irá estornar os r$ 13,20 e cobrar só os r$ 7,63 (como está descrito no recibo abaixo enviado ao meu email) ou a @uber_brasil irá devolver os meus r$ 5,57 de créditos e deixar o valor integral da corrida no meu cartão</t>
+  </si>
+  <si>
+    <t>@capinadaqui lembrei do cara do uber skkskskssk</t>
+  </si>
+  <si>
+    <t>@hbredda bredda, se a vida te dá limões, faça uma limonada. imagina como estará o transito de sp nesses dias.. vou aproveitar que estou de home office e fazer uns bicos de uber</t>
+  </si>
+  <si>
+    <t>@amywinehazi se fosse uber https://t.co/7bmj21vy9r</t>
+  </si>
+  <si>
+    <t>rt @fvckyovxx: uber do minguito é o homem de ferro</t>
+  </si>
+  <si>
+    <t>tocando sambinha no uber muito bom dia sim</t>
+  </si>
+  <si>
+    <t>to mal acostumado indo de uber trabalhar todo dia</t>
+  </si>
+  <si>
+    <t>rt @crvglucao_: se eu fosse uber
+*passageiro tosse* 
+eu:</t>
+  </si>
+  <si>
+    <t>@_camilym @que_stefany a gente vai começar a só ir de uber nos lugares agora</t>
+  </si>
+  <si>
+    <t>maluco...
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro visite perfil https://t.co/kegtujidhh</t>
+  </si>
+  <si>
+    <t>@estadao @mariacidada1 "seu abandono será o alimento dos vírus q invadirão as trincheiras da classe média, virão pelo ar, como anjos vingadores, trazidos pela empregada..q ñ será dispensada..entregadores..seguranças..uber..babá.. a coronavirus..antecipou a catástrofe provinda do fim da solidariedade.."</t>
+  </si>
+  <si>
+    <t>rt @hobibabiee: audios para quando você se sentir desconfortavel no uber/99 a thread https://t.co/gwnqrjjhef</t>
+  </si>
+  <si>
+    <t>o quão adolescente padrão você é?
+tem netflix: 👎
+tem spotify: 👎
+tem telecine p: 👎
+tem crush: 👍
+tem mais de 5 amgs: 👍
+é popular: 👎
+tem iphone: 👎
+tem android: 👍
+tem mais de 1,50: 👍
+é mimade: 👍
+a família é unida: 👎
+tem um quarto só seu: 👎
+anda de uber: 👎 https://t.co/mxbwr90zyv</t>
+  </si>
+  <si>
+    <t>@gabiivieirar @vitornoisvai @uber_brasil seu marido deve ser de boa índole mas existem pessoas que não. de qualquer forma ele deve saber que quando o cliente descer ele deve encerrar a corrida. caso contrário causa muito transtorno. se ele estivesse trabalhando numa empresa isso seria um erro gravíssimo.</t>
+  </si>
+  <si>
+    <t>rt @edgardrago14: quem vai lucrar imenso com esta quarentena vai ser a uber eats</t>
+  </si>
+  <si>
+    <t>eu limpo os mínimos detalhes do carro do meu pai, para que os passageiros dele se sintam bem e confortáveis tendo o serviço dele, pq cara é oque tds nos queremos. porém, eu entro em uns carros da uber que ptm, sem condições!</t>
+  </si>
+  <si>
+    <t>@normose_ esse uber vai um dia pegar um carona vírus</t>
+  </si>
+  <si>
+    <t>oa lixo, que acha que os 6 reais que ele paga, é o aluguel de uma limousine, com direito a tapete vermelho e cerveja gratis, e ainda tem gente que tem "medo de andar sozinha"
+madame, ande de uber que eu garanto que isso não acontece, se acontecer você tem o áudio da corrida grava</t>
+  </si>
+  <si>
+    <t>rt @akaliuchis: imaginando o uber ouvindo o mesmo áudio pela 10° vez  https://t.co/tjkxtsqvqv</t>
+  </si>
+  <si>
+    <t>rt @sltisfaction: merda do corona, eu tinha bue descontos esta semana na uber eats</t>
+  </si>
+  <si>
+    <t>@maramandrea brigado pelas dicas mana querida! sim, eu tenho fotografado mais nas ruas mesmo e caminhando mais que usando transporte público ou uber
+qual o tipo de máscara que eu devia comprar? me fala que eu tô querendo mesmo ter uma, nem sempre posso fugir do metrô..ônibus é mas tranquilo</t>
+  </si>
+  <si>
+    <t>tá procurando isso que eu sei!
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro visite o nosso perfil https://t.co/dqfxpjcfmc</t>
+  </si>
+  <si>
+    <t>@davisss89 @erickwillsx não estrague a ideia da quarentena, o uber passou álcool em gel na mão ok</t>
+  </si>
+  <si>
+    <t>o auge o uber fzd eu mostrar a identidade pq ele nao leva menor de idade kkkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>cupom uber março 2020 - ganhe duas corridas na faixa! baixe o aplicativo e use o código: prpon9 https://t.co/lycyawpcxc</t>
+  </si>
+  <si>
+    <t>homem nenhum sabe como a gente precisa disso se estivermos sozinhas no uber https://t.co/fnrlhow3em</t>
+  </si>
+  <si>
+    <t>vontade de dar um espirro no uber mas com medo de ser largada no meio do caminho</t>
+  </si>
+  <si>
+    <t>@aafroditeee @uber_brasil muito ruim uma mulher ter que justificar uma frase numa conversa pra um homem nojento que entende o que quer e leva pro lado que quer só pq é desconfortável. por menos eu mandava tomar no cu</t>
+  </si>
+  <si>
+    <t>@cruelladejinx @fckjergui @insensatafada aqui n tem uber  🤭🤭🤭</t>
+  </si>
+  <si>
+    <t>nico veio falando um língua totalmente nova no uber kkkjkkk eu amo</t>
+  </si>
+  <si>
+    <t>meu white people problem de hoje é que uma hora dessas eu to pesquisando como que anda de ônibus em santos pq vou ter que parar de andar de uber pra realmente conhecer a cidade 😩</t>
+  </si>
+  <si>
+    <t>rt @arthurmoledoval: sp tem vários problemas reais: enchentes, trânsito, regularização fundiária, saneamento, roubo...
+mas parte dos verea…</t>
+  </si>
+  <si>
+    <t>se ele sai de role e fica doidasso e ainda manda áudio gravando a conversa com o uber falando de vc como se fosse a mulher maravilha: eh ele</t>
+  </si>
+  <si>
+    <t>pra variar, uns motora da @uber_brasil cancelando corrida por ser no cartão de crédito. https://t.co/j4z8lk9gvu</t>
+  </si>
+  <si>
+    <t>rt @sacardcaptor: tô tão titi alguém me manda cupom do uber eats @ubereats_br :(</t>
+  </si>
+  <si>
+    <t>rt @fdinizspfc: obrigado pela moral, uber! 👍🏼 https://t.co/pxt8haqgot</t>
+  </si>
+  <si>
+    <t>queria saber qual o prazer desse uber aceitar minha corrida me mandar uma mensagem falando "olá vou ser seu motorista, qual o destino" ai eu falei ele cancelou</t>
+  </si>
+  <si>
+    <t>nossa gente, esses áudios de "se sentir desconfortável no uber use" aqui no rj não ia adiantar muito não, tem que fazer voz de pai ou mãe gritando brigando "filho da p* cadê você caralh*? localização ok, quando chegar em casa vai tomar uma surra, to esperando no portão" aí sim!!!</t>
+  </si>
+  <si>
+    <t>o motorista do uber tentando me convencer que o corona vírus foi criado pelos ricos para dizimar a população periférica dos países subdesenvolvidos.
+“se isso entra um uma prisão mata todo mundo e eu não acho isso ruim” https://t.co/1affxkqz6l</t>
+  </si>
+  <si>
+    <t>@vitornoisvai @uber_brasil aí é difícil viu. não entendo pq eles fazem isso.</t>
+  </si>
+  <si>
+    <t>pedi um uber pra deixar o otavio em casa
+era a uber que ele tinha gorfado no carro uma vez</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/caksxbyaqr</t>
+  </si>
+  <si>
+    <t>rt @fvckyovxx: uber do minguito é o homem de ferro https://t.co/txicpxbbyp</t>
+  </si>
+  <si>
+    <t>não tô gostando desse uber</t>
+  </si>
+  <si>
+    <t>achei que tinha pedido o uber no cartão, pedi no dinheiro e o sufuco pra pagar o homem as 6 da manhã  kkkk</t>
+  </si>
+  <si>
+    <t>depois de baterem palmas ao sns aconselho também baterem palmas mas aos gajos da glovo e da uber que continuam a entregar comida por aí #covidー19</t>
+  </si>
+  <si>
+    <t>@marleneffl @patriaamada_br @marciom02035740 vá de ônibus, vá de máscara, vá a pé, vá de táxi ou de uber, mas vá. o brasil agradece.
+#bolsonaroday</t>
+  </si>
+  <si>
+    <t>rt @liaamancio: coronafest.
+não tenho pena, mas amanhã esse bando de arrombado vai transmitir pra caixa do supermercado, pro motorista do…</t>
+  </si>
+  <si>
+    <t>entrei no uber e tava tocando luan santana, tive q pedir pra trocar</t>
+  </si>
+  <si>
+    <t>@hoseokpassiva ei eu pago seu uber coisa linda 😘</t>
+  </si>
+  <si>
+    <t>olha aí seu presentim :)
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas amazon, airbnb, recargapay, mercado livre, pagseguro lá no perfil! https://t.co/bvruihbohs</t>
+  </si>
+  <si>
+    <t>rt @codebywoman: meu amigo me convencendo da ideia de “uber de sei la oq” que ele não precisa validar e já tem certeza q vai nos deixar ric…</t>
+  </si>
+  <si>
+    <t>uber eats vc me prometeu entrega grátis</t>
+  </si>
+  <si>
+    <t>gente nunca me senti tão desconfortável dentro de um uber, sério q nojo 🤢🤮</t>
+  </si>
+  <si>
+    <t>to apaixonada no uber ô caiçara fofo</t>
+  </si>
+  <si>
+    <t>[15/3 10:36] dançarino preferido: eu q te ajudei a colocar o short, te enfiei no uber 
+catei tuas coisas
+[15/3 10:36] dançarino preferido: foi de short
+o patrick é o amr da minha vida kkkkkkjkkkkkkk</t>
+  </si>
+  <si>
+    <t>meu 99 não tá pegando de jeito nenhum quero vê eu arrumar um uber pra ir p casa nessa porra</t>
+  </si>
+  <si>
+    <t>gente o meu uber ontem era pft
+tinha balinha, uma caixa térmica com água, álcool em gel, ar condicionado e várias instruções de como avaliar ele (se ele correu em uma velocidade boa, 1 estrela, se ele foi educado, +1 estrela, e assim até formar 5 estrelas)</t>
+  </si>
+  <si>
+    <t>de nada pessoal kkk aproveitem ;)
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas amazon, airbnb, recargapay, mercado livre, pagseguro lá no perfil! https://t.co/qpho4o6kex</t>
+  </si>
+  <si>
+    <t>o rolê de ontem foi ótimo 
+&amp;gt; não paguei uber de ida
+&amp;gt; não paguei ingresso pois ganhei no sorteio
+&amp;gt; teve open, não gastei com bebida (só água, hidratadah)
+tudo viu, compensou os outros que gastei horrores</t>
+  </si>
+  <si>
+    <t>o uber de ontem foi perfeito</t>
+  </si>
+  <si>
+    <t>ontem no uber o cara nao quis ligar o ar por causa do corona, fui derretendo mesmo, cheguei no shopping todo suado</t>
+  </si>
+  <si>
+    <t>uber em bc é uma merda</t>
+  </si>
+  <si>
+    <t>@clarckhammer ai amigo eu também achava que não conseguia masss ontem não tava afim mesmo de ficar louca e ngm que tava lá comigo morava perto de casa, então eu teria que entrar num uber sozinha, aí acho que isso me ajudou a controlar</t>
+  </si>
+  <si>
+    <t>rt @saymonsn777: mano eu @emillymeneli e @marcosjaquesmj no uber com uns papo de futuro, estudo, trabalho, será-se tamo virando gente? kaka…</t>
+  </si>
+  <si>
+    <t>ontem eu morri de medo quando peguei uber e ele disse que eu tinha voz daquele programa que tinha na rádio, o disk sexo, e ficou perguntando se eu tinha namorado o cu não passava uma linha</t>
+  </si>
+  <si>
+    <t>@biakru eu até pesquisei no uber eats mas não tinha como, era pizza ou sanduíche só que entregava</t>
+  </si>
+  <si>
+    <t>o quão adolescente padrão você é?
+tem netflix: ✅
+tem spotify: ✅ 
+tem telecine p: ✅
+tem crush: ❌
+tem mais de 5 amgs:✅
+é popular: ❌
+tem iphone: ✅
+tem android: ❌
+tem mais de 1,50: ✅
+é mimade: ❌✅
+a família é unida:❌
+tem um quarto só seu: ❌
+anda de uber: ✅ https://t.co/v1ywhje8nc</t>
+  </si>
+  <si>
+    <t>uber em arraial tocando 1d simplesmente perfeito</t>
+  </si>
+  <si>
+    <t>rt @clubedosfamosos: #bolsonaroday será o dia que vou pagar pra manifestar!
+copacabana a cerva é 10 real, tem uber, camiseta, boné, bandeir…</t>
+  </si>
+  <si>
+    <t>agra tem que segurar a tosse no uber</t>
+  </si>
+  <si>
+    <t>toma lá:
+cupom do ifood (app) =&amp;gt; ee6hz487al
+código rappi =&amp;gt; 82q38640354
+uber -&amp;gt; rjefc5
+r$ 10,00 picpay =&amp;gt; hjsw1z
+99 (carona) -&amp;gt; s53bdg5a
+ desconto uber eats =&amp;gt; eats-rjefc5
+ofertas da amazon, airbnb, recargapay, mercado livre e pagseguro no perfil! https://t.co/2tocjjvrku</t>
+  </si>
+  <si>
+    <t>eu fiz boa noite pro uber</t>
+  </si>
+  <si>
+    <t>rt @tonkiel: imagina que nesse avião tenha, sei lá, umas 300 pessoas. digamos que a metade use uber pra sair do aeroporto. se 2 estiverem i…</t>
+  </si>
+  <si>
+    <t>entrei no uber, dei boa noite.
+o motorista: " nossa, que cheiro de cachaça"
+mano! queria me enfiar num buraco, que vergonha</t>
+  </si>
+  <si>
+    <t>kkkkkk o uber dando em cima da minha mãe</t>
+  </si>
+  <si>
+    <t>+30 graus por aqui....
+e ainda ter que pedir/implorar pros motoristas da @uber_brasil e @voude99 ligarem o ar condicionado.</t>
+  </si>
+  <si>
+    <t>@folieakilljoy eita porra???? tu vai de uber? hsjdisydd
+e eu aqui reclamando que pago 3,65</t>
+  </si>
+  <si>
+    <t>rt @oodiodobem: uber protegido de todos os corongas vírus https://t.co/wyxjlu4jya</t>
+  </si>
+  <si>
+    <t>@uber_support @ellecramm mais uma palhaçada, segue a gente, agora eu que sigo esse lixo de empresa não recebo o que me devem, más o importante é terem seguidores, o empresa lixo, paga ninguém , más seguidores eles querem.</t>
+  </si>
+  <si>
+    <t>@camilaeuzebio_ @procurandotory pega um uber pra rodoviária e vai de ônibus kkkkkkk ou se ficar mais barato vai de ubi mesmo</t>
+  </si>
+  <si>
+    <t>queria saber qual cartão eu botei no uber kkkkkk e quem vai pagar tbm kkk</t>
+  </si>
+  <si>
+    <t>vem de uber q eu pago</t>
+  </si>
+  <si>
+    <t>rt @brunofiocchi: quer um sinal de compra forte? entrar no uber e o motorista falar que esta short em bolsa.</t>
+  </si>
+  <si>
+    <t>ontem eu quase paguei 38 reais no uber pra ir dormir com o perturbado, mas se eu fosse eu ia me sentir muito usada. 
+ainda bem que a mamis dele mandou ele entrar kkkkkk</t>
+  </si>
+  <si>
+    <t>cupons de desconto
+rappi
+hrp32015999 - 150 em frete grátis + 20 com google pay
+recargapay:
+matr698 - ganhe 10 reais para pagar boleto ou recarga.
+ifood:
+p8n9n9smwb - 20 reais no seu primeiro pedido
+99 cupom
+br6e2332 - ganhe 15 reais na sua corrida.
+uber -  vx453h https://t.co/rczfaqkgcw</t>
+  </si>
+  <si>
+    <t>muito importante pra vcs q andam de uber migos... https://t.co/554dhhiviu</t>
+  </si>
+  <si>
+    <t>rt @prodrigo434: o rico passa férias em milão. volta e transmite coronavirus pro uber. o rico fica na quarentena com todo conforto, vivendo…</t>
+  </si>
+  <si>
+    <t>o amra esqueceu o cooler no uber puta que o pariu</t>
+  </si>
+  <si>
+    <t>11h é o casamento, 11h tô pegando o uber kkkkkkkkk</t>
+  </si>
+  <si>
+    <t>odeio andar de uber, todos tem cheiro ruim</t>
+  </si>
+  <si>
+    <t>@celomado a volta pra casa, tive que ir pra praia grande pra conseguir um uber</t>
+  </si>
+  <si>
+    <t>meu irmao eh uber vo fala p ele faze isso https://t.co/4sg5rgwclt</t>
+  </si>
+  <si>
+    <t>espirrei no uber e o motorista começou a passar álcool na mão, calma parça é só um coroninha</t>
+  </si>
+  <si>
+    <t>ainda n acredito q pagamos 50 conto no uber</t>
+  </si>
+  <si>
+    <t>rt @eurafaas: eu não faço ideia de como é ser mulher, mas escutando esse áudio eu fiquei triste a ponto de perceber que a mulher tem coloca…</t>
+  </si>
+  <si>
+    <t>@barb_lanzarin não!! espera que eu vou chamar o uber.</t>
+  </si>
+  <si>
+    <t>@olimpiabarbara @uber_brasil pois é, o cara só finalizou quando eu liguei a décima vez pelo app</t>
+  </si>
+  <si>
+    <t>eu gritando com o uber toda vez que alguma amiga sai da minha casa https://t.co/tp1pcoqjvq</t>
+  </si>
+  <si>
+    <t>@paoherco1 @esmareana @fercoboen @_juliocalderon pedimos taquitos por uber eats.</t>
+  </si>
+  <si>
+    <t>peguei um uber agora e o motorista começou a tossir do meu lado, pedi pra desligar o ar e abrir a janela.</t>
+  </si>
+  <si>
+    <t>thread de vídeos para usar no uber/99 quando estiver se sentindo desconfortável ou algo assim ❤️</t>
+  </si>
+  <si>
+    <t>rt @universitariaof: e o uber que se protegeu do corona vírus com plástico filme no carro?????? kkkkkkkk https://t.co/0sodyngbtv</t>
+  </si>
+  <si>
+    <t>@quebrachera eu penso no meu pai q não consegue se aposentar e tem q fazer uber e tenho vontade de estrangular com as minhas próprias mãos</t>
+  </si>
+  <si>
+    <t>e ainda teve cara de pau de dar cartãozinho dele de uber kkkk a</t>
+  </si>
+  <si>
+    <t>minha mãe bebeu ousadia pra crc ontem que falou pra eu pedir uber com copo descartável 🤦🏽‍♂️🤣🤣🤣</t>
   </si>
 </sst>
 </file>
@@ -2278,9 +3064,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A473" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E304" sqref="E304"/>
     </sheetView>
   </sheetViews>
@@ -4594,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -4602,7 +5388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -4610,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -4618,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>291</v>
       </c>
@@ -4626,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>292</v>
       </c>
@@ -4634,7 +5420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>293</v>
       </c>
@@ -4642,7 +5428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>294</v>
       </c>
@@ -4650,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>295</v>
       </c>
@@ -4658,7 +5444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>296</v>
       </c>
@@ -4666,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -4674,7 +5460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>298</v>
       </c>
@@ -4682,7 +5468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -4690,11 +5476,1612 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>300</v>
       </c>
       <c r="B301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>503</v>
+      </c>
+      <c r="B302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>504</v>
+      </c>
+      <c r="B303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>505</v>
+      </c>
+      <c r="B304">
+        <v>0</v>
+      </c>
+      <c r="E304" s="3"/>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>506</v>
+      </c>
+      <c r="B305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>507</v>
+      </c>
+      <c r="B306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>508</v>
+      </c>
+      <c r="B307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>509</v>
+      </c>
+      <c r="B308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>510</v>
+      </c>
+      <c r="B309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>511</v>
+      </c>
+      <c r="B310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>512</v>
+      </c>
+      <c r="B311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>513</v>
+      </c>
+      <c r="B312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>514</v>
+      </c>
+      <c r="B313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>515</v>
+      </c>
+      <c r="B314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>516</v>
+      </c>
+      <c r="B315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>517</v>
+      </c>
+      <c r="B316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>518</v>
+      </c>
+      <c r="B317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>519</v>
+      </c>
+      <c r="B318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>520</v>
+      </c>
+      <c r="B319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>521</v>
+      </c>
+      <c r="B320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>522</v>
+      </c>
+      <c r="B321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
+        <v>523</v>
+      </c>
+      <c r="B322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>524</v>
+      </c>
+      <c r="B323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>525</v>
+      </c>
+      <c r="B324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>526</v>
+      </c>
+      <c r="B325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>527</v>
+      </c>
+      <c r="B326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>528</v>
+      </c>
+      <c r="B327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>529</v>
+      </c>
+      <c r="B328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>530</v>
+      </c>
+      <c r="B329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>531</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>532</v>
+      </c>
+      <c r="B331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>533</v>
+      </c>
+      <c r="B332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>534</v>
+      </c>
+      <c r="B333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>535</v>
+      </c>
+      <c r="B334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>536</v>
+      </c>
+      <c r="B335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>537</v>
+      </c>
+      <c r="B336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>538</v>
+      </c>
+      <c r="B337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>539</v>
+      </c>
+      <c r="B338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>540</v>
+      </c>
+      <c r="B339">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>541</v>
+      </c>
+      <c r="B340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>542</v>
+      </c>
+      <c r="B341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>543</v>
+      </c>
+      <c r="B342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>544</v>
+      </c>
+      <c r="B343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>545</v>
+      </c>
+      <c r="B344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>546</v>
+      </c>
+      <c r="B345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>547</v>
+      </c>
+      <c r="B346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>548</v>
+      </c>
+      <c r="B347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>549</v>
+      </c>
+      <c r="B348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>550</v>
+      </c>
+      <c r="B349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>551</v>
+      </c>
+      <c r="B350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>552</v>
+      </c>
+      <c r="B351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>553</v>
+      </c>
+      <c r="B352">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>554</v>
+      </c>
+      <c r="B353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>555</v>
+      </c>
+      <c r="B354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>556</v>
+      </c>
+      <c r="B355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>557</v>
+      </c>
+      <c r="B356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>558</v>
+      </c>
+      <c r="B357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>559</v>
+      </c>
+      <c r="B358">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>560</v>
+      </c>
+      <c r="B359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>561</v>
+      </c>
+      <c r="B360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>562</v>
+      </c>
+      <c r="B361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>563</v>
+      </c>
+      <c r="B362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>564</v>
+      </c>
+      <c r="B363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>565</v>
+      </c>
+      <c r="B364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>566</v>
+      </c>
+      <c r="B365">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>567</v>
+      </c>
+      <c r="B366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>568</v>
+      </c>
+      <c r="B367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>569</v>
+      </c>
+      <c r="B368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>570</v>
+      </c>
+      <c r="B369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>571</v>
+      </c>
+      <c r="B370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>572</v>
+      </c>
+      <c r="B371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>573</v>
+      </c>
+      <c r="B372">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>574</v>
+      </c>
+      <c r="B373">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>575</v>
+      </c>
+      <c r="B374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>576</v>
+      </c>
+      <c r="B375">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>577</v>
+      </c>
+      <c r="B376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>578</v>
+      </c>
+      <c r="B377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>579</v>
+      </c>
+      <c r="B378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>580</v>
+      </c>
+      <c r="B379">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>581</v>
+      </c>
+      <c r="B380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>582</v>
+      </c>
+      <c r="B381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>583</v>
+      </c>
+      <c r="B382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>584</v>
+      </c>
+      <c r="B383">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>585</v>
+      </c>
+      <c r="B384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>586</v>
+      </c>
+      <c r="B385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>587</v>
+      </c>
+      <c r="B386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>588</v>
+      </c>
+      <c r="B387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>589</v>
+      </c>
+      <c r="B388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>590</v>
+      </c>
+      <c r="B389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>591</v>
+      </c>
+      <c r="B390">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>592</v>
+      </c>
+      <c r="B391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>593</v>
+      </c>
+      <c r="B392">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>594</v>
+      </c>
+      <c r="B393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>595</v>
+      </c>
+      <c r="B394">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>596</v>
+      </c>
+      <c r="B395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>597</v>
+      </c>
+      <c r="B396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>598</v>
+      </c>
+      <c r="B397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>599</v>
+      </c>
+      <c r="B398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>600</v>
+      </c>
+      <c r="B399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>601</v>
+      </c>
+      <c r="B400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>602</v>
+      </c>
+      <c r="B401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>603</v>
+      </c>
+      <c r="B402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>604</v>
+      </c>
+      <c r="B403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>605</v>
+      </c>
+      <c r="B404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A405" t="s">
+        <v>606</v>
+      </c>
+      <c r="B405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>607</v>
+      </c>
+      <c r="B406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>608</v>
+      </c>
+      <c r="B407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>609</v>
+      </c>
+      <c r="B408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>610</v>
+      </c>
+      <c r="B409">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>611</v>
+      </c>
+      <c r="B410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>612</v>
+      </c>
+      <c r="B411">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>613</v>
+      </c>
+      <c r="B412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>614</v>
+      </c>
+      <c r="B413">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>615</v>
+      </c>
+      <c r="B414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>616</v>
+      </c>
+      <c r="B415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>617</v>
+      </c>
+      <c r="B416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>618</v>
+      </c>
+      <c r="B417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>619</v>
+      </c>
+      <c r="B418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>620</v>
+      </c>
+      <c r="B419">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>621</v>
+      </c>
+      <c r="B420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>622</v>
+      </c>
+      <c r="B421">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>623</v>
+      </c>
+      <c r="B422">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>624</v>
+      </c>
+      <c r="B423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>625</v>
+      </c>
+      <c r="B424">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>626</v>
+      </c>
+      <c r="B425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>627</v>
+      </c>
+      <c r="B426">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>628</v>
+      </c>
+      <c r="B427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>629</v>
+      </c>
+      <c r="B428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>630</v>
+      </c>
+      <c r="B429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>631</v>
+      </c>
+      <c r="B430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>632</v>
+      </c>
+      <c r="B431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>633</v>
+      </c>
+      <c r="B432">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>634</v>
+      </c>
+      <c r="B433">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>635</v>
+      </c>
+      <c r="B434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>636</v>
+      </c>
+      <c r="B435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>637</v>
+      </c>
+      <c r="B436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>638</v>
+      </c>
+      <c r="B437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>639</v>
+      </c>
+      <c r="B438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>640</v>
+      </c>
+      <c r="B439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>641</v>
+      </c>
+      <c r="B440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>642</v>
+      </c>
+      <c r="B441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>643</v>
+      </c>
+      <c r="B442">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>644</v>
+      </c>
+      <c r="B443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>645</v>
+      </c>
+      <c r="B444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>646</v>
+      </c>
+      <c r="B445">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>647</v>
+      </c>
+      <c r="B446">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>648</v>
+      </c>
+      <c r="B447">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>649</v>
+      </c>
+      <c r="B448">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>650</v>
+      </c>
+      <c r="B449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>651</v>
+      </c>
+      <c r="B450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>652</v>
+      </c>
+      <c r="B451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>653</v>
+      </c>
+      <c r="B452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>654</v>
+      </c>
+      <c r="B453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>655</v>
+      </c>
+      <c r="B454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>656</v>
+      </c>
+      <c r="B455">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>657</v>
+      </c>
+      <c r="B456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>658</v>
+      </c>
+      <c r="B457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>659</v>
+      </c>
+      <c r="B458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>660</v>
+      </c>
+      <c r="B459">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>661</v>
+      </c>
+      <c r="B460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>662</v>
+      </c>
+      <c r="B461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A462" t="s">
+        <v>663</v>
+      </c>
+      <c r="B462">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A463" t="s">
+        <v>664</v>
+      </c>
+      <c r="B463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A464" t="s">
+        <v>665</v>
+      </c>
+      <c r="B464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A465" t="s">
+        <v>666</v>
+      </c>
+      <c r="B465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A466" t="s">
+        <v>667</v>
+      </c>
+      <c r="B466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A467" t="s">
+        <v>668</v>
+      </c>
+      <c r="B467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A468" t="s">
+        <v>669</v>
+      </c>
+      <c r="B468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A469" t="s">
+        <v>670</v>
+      </c>
+      <c r="B469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A470" t="s">
+        <v>671</v>
+      </c>
+      <c r="B470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A471" t="s">
+        <v>672</v>
+      </c>
+      <c r="B471">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A472" t="s">
+        <v>673</v>
+      </c>
+      <c r="B472">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A473" t="s">
+        <v>674</v>
+      </c>
+      <c r="B473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A474" t="s">
+        <v>675</v>
+      </c>
+      <c r="B474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A475" t="s">
+        <v>676</v>
+      </c>
+      <c r="B475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A476" t="s">
+        <v>677</v>
+      </c>
+      <c r="B476">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A477" t="s">
+        <v>678</v>
+      </c>
+      <c r="B477">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A478" t="s">
+        <v>679</v>
+      </c>
+      <c r="B478">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A479" t="s">
+        <v>680</v>
+      </c>
+      <c r="B479">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A480" t="s">
+        <v>681</v>
+      </c>
+      <c r="B480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A481" t="s">
+        <v>682</v>
+      </c>
+      <c r="B481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A482" t="s">
+        <v>683</v>
+      </c>
+      <c r="B482">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A483" t="s">
+        <v>684</v>
+      </c>
+      <c r="B483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A484" t="s">
+        <v>685</v>
+      </c>
+      <c r="B484">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A485" t="s">
+        <v>686</v>
+      </c>
+      <c r="B485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A486" t="s">
+        <v>687</v>
+      </c>
+      <c r="B486">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A487" t="s">
+        <v>688</v>
+      </c>
+      <c r="B487">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A488" t="s">
+        <v>689</v>
+      </c>
+      <c r="B488">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A489" t="s">
+        <v>690</v>
+      </c>
+      <c r="B489">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A490" t="s">
+        <v>691</v>
+      </c>
+      <c r="B490">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>692</v>
+      </c>
+      <c r="B491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>693</v>
+      </c>
+      <c r="B492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>694</v>
+      </c>
+      <c r="B493">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>695</v>
+      </c>
+      <c r="B494">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>696</v>
+      </c>
+      <c r="B495">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A496" t="s">
+        <v>697</v>
+      </c>
+      <c r="B496">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A497" t="s">
+        <v>698</v>
+      </c>
+      <c r="B497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>699</v>
+      </c>
+      <c r="B498">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A499" t="s">
+        <v>700</v>
+      </c>
+      <c r="B499">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A500" t="s">
+        <v>701</v>
+      </c>
+      <c r="B500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A501" t="s">
+        <v>702</v>
+      </c>
+      <c r="B501">
         <v>0</v>
       </c>
     </row>
@@ -4708,7 +7095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A166" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>